<commit_message>
add tcp server example
</commit_message>
<xml_diff>
--- a/examples/webapp/tables/partTable.xlsx
+++ b/examples/webapp/tables/partTable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\go\src\github.com\nekohor\gomon\examples\app\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nekohor\go\src\github.com\nekohor\gomon\examples\webapp\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="50511" yWindow="0" windowWidth="17197" windowHeight="6217"/>
+    <workbookView xWindow="51435" yWindow="0" windowWidth="17190" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="406">
   <si>
     <t>LINE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1496,15 +1496,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>os_bend_force7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TN\\L2_FA_FDT1TEMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>os_bend_force1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>os_bend_force7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TN\\L2_FA_FDT1TEMP</t>
+    <t>wedge70</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2019,11 +2023,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.75" style="3"/>
     <col min="2" max="2" width="22.25" style="3" bestFit="1" customWidth="1"/>
@@ -2275,7 +2279,7 @@
         <v>1580</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>318</v>
+        <v>405</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>297</v>
@@ -3443,7 +3447,7 @@
         <v>309</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
@@ -5061,7 +5065,7 @@
         <v>1580</v>
       </c>
       <c r="B221" s="11" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C221" s="11" t="s">
         <v>298</v>
@@ -5243,7 +5247,7 @@
         <v>2250</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C234" s="14" t="s">
         <v>304</v>

</xml_diff>